<commit_message>
try to improve the different id columns in the dataset: now there's a group id column for tying parents & children together (generated from mods id if missing), a mods id column (mods id is generated from group id if missing), and a file name column that names the datafile (and isn't used for the other ids)
</commit_message>
<xml_diff>
--- a/test_files/data.xlsx
+++ b/test_files/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="161"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="15560" tabRatio="161" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="71">
   <si>
     <t>Media Title</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>do not map</t>
-  </si>
-  <si>
-    <t>record name</t>
   </si>
   <si>
     <r>
@@ -273,6 +270,12 @@
   </si>
   <si>
     <t>Test Note 2</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>group id</t>
   </si>
 </sst>
 </file>
@@ -773,11 +776,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:33" s="9" customFormat="1" ht="18.25" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -888,83 +891,83 @@
         <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="X2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="AC2" s="6" t="s">
         <v>33</v>
       </c>
@@ -978,18 +981,18 @@
         <v>33</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="14" customFormat="1" ht="17" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="12">
         <v>123</v>
@@ -1002,58 +1005,58 @@
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="L3" s="16">
         <v>38646</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O3" s="18">
         <v>123</v>
       </c>
       <c r="P3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="R3" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>55</v>
       </c>
       <c r="S3" s="19"/>
       <c r="T3" s="19"/>
       <c r="U3" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="W3" s="20">
         <v>38635</v>
       </c>
       <c r="X3" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y3" s="19"/>
       <c r="Z3" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="AB3" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="AC3" s="19"/>
       <c r="AD3" s="19"/>
@@ -1063,13 +1066,13 @@
     </row>
     <row r="4" spans="1:33" s="14" customFormat="1" ht="16.25" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10">
         <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="12">
         <v>234</v>
@@ -1082,58 +1085,58 @@
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>64</v>
       </c>
       <c r="L4" s="22">
         <v>38646</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O4" s="18">
         <v>234</v>
       </c>
       <c r="P4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="19" t="s">
-        <v>54</v>
-      </c>
       <c r="R4" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S4" s="19"/>
       <c r="T4" s="19"/>
       <c r="U4" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V4" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="W4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="20" t="s">
-        <v>68</v>
-      </c>
       <c r="X4" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y4" s="19"/>
       <c r="Z4" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA4" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB4" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="AB4" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="AC4" s="19"/>
       <c r="AD4" s="19"/>
@@ -1160,11 +1163,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:33" s="9" customFormat="1" ht="18.25" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -1275,83 +1278,83 @@
         <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="X2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="AC2" s="6" t="s">
         <v>33</v>
       </c>
@@ -1365,18 +1368,18 @@
         <v>33</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="14" customFormat="1" ht="17" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="12">
         <v>123</v>
@@ -1389,58 +1392,58 @@
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="L3" s="16">
         <v>39742</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O3" s="18">
         <v>123</v>
       </c>
       <c r="P3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="R3" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>55</v>
       </c>
       <c r="S3" s="19"/>
       <c r="T3" s="19"/>
       <c r="U3" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="W3" s="20">
         <v>38635</v>
       </c>
       <c r="X3" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y3" s="19"/>
       <c r="Z3" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="AB3" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="AC3" s="19"/>
       <c r="AD3" s="19"/>
@@ -1469,7 +1472,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>